<commit_message>
Added filter by geo on collecting cript
</commit_message>
<xml_diff>
--- a/reports/indicators.xlsx
+++ b/reports/indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor.latii\Desktop\AED_lab_1\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAF64F1-AB84-4F69-9036-E100BAC62021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753265E7-C8EA-4026-9330-B2E4ABD5625E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2205" windowWidth="25110" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
   <si>
     <t>Code</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>Selected Indicators for Assignment 1</t>
+  </si>
+  <si>
+    <t>Used for RQ</t>
+  </si>
+  <si>
+    <t>RQ1</t>
+  </si>
+  <si>
+    <t>RQ3</t>
+  </si>
+  <si>
+    <t>RQ1, RQ3</t>
+  </si>
+  <si>
+    <t>RQ2</t>
   </si>
 </sst>
 </file>
@@ -324,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -336,13 +351,12 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -623,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57396EAD-0A46-44EE-9AAA-FBAB859B9C70}">
-  <dimension ref="A2:G29"/>
+  <dimension ref="A2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,20 +651,21 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -672,8 +687,11 @@
       <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -695,8 +713,11 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -718,8 +739,11 @@
       <c r="G6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -741,8 +765,11 @@
       <c r="G7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -764,8 +791,11 @@
       <c r="G8" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -787,8 +817,11 @@
       <c r="G9" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -810,9 +843,12 @@
       <c r="G10" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="H10" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -833,8 +869,11 @@
       <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -856,8 +895,11 @@
       <c r="G12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -879,8 +921,11 @@
       <c r="G13" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -902,8 +947,11 @@
       <c r="G14" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>11</v>
       </c>
@@ -925,8 +973,11 @@
       <c r="G15" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H15" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>12</v>
       </c>
@@ -948,8 +999,11 @@
       <c r="G16" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>13</v>
       </c>
@@ -971,8 +1025,11 @@
       <c r="G17" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -994,8 +1051,11 @@
       <c r="G18" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>15</v>
       </c>
@@ -1017,9 +1077,12 @@
       <c r="G19" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="6"/>
+      <c r="H19" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>